<commit_message>
fix read input file, add exe
</commit_message>
<xml_diff>
--- a/input/input.xlsx
+++ b/input/input.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -34,6 +34,18 @@
   </si>
   <si>
     <t>SOL-USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tether USDt</t>
+  </si>
+  <si>
+    <t>USDT-USD</t>
+  </si>
+  <si>
+    <t>XRP</t>
+  </si>
+  <si>
+    <t>XRP-USD</t>
   </si>
 </sst>
 </file>
@@ -613,6 +625,28 @@
         <v>6</v>
       </c>
       <c r="C3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
         <v>2000</v>
       </c>
     </row>

</xml_diff>